<commit_message>
Adjust measurement validation and update pressure calculations in wvpweerstand.py
</commit_message>
<xml_diff>
--- a/productiecapaciteit/results/Wvpweerstand/Wvpweerstand_modelcoefficienten.xlsx
+++ b/productiecapaciteit/results/Wvpweerstand/Wvpweerstand_modelcoefficienten.xlsx
@@ -497,7 +497,7 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>-0.01421624178035649</v>
+        <v>-0.01436667179288742</v>
       </c>
     </row>
     <row r="3">
@@ -517,7 +517,7 @@
         </is>
       </c>
       <c r="B4" t="n">
-        <v>-9.456167332204952e-07</v>
+        <v>-8.046470117331002e-07</v>
       </c>
     </row>
     <row r="5">
@@ -527,7 +527,7 @@
         </is>
       </c>
       <c r="B5" t="n">
-        <v>11.90303794667552</v>
+        <v>12.4336236677692</v>
       </c>
     </row>
     <row r="6">
@@ -537,7 +537,7 @@
         </is>
       </c>
       <c r="B6" t="n">
-        <v>6.689706176707028</v>
+        <v>7.109866935233991</v>
       </c>
     </row>
     <row r="7">
@@ -547,7 +547,7 @@
         </is>
       </c>
       <c r="B7" t="n">
-        <v>160.0007830196669</v>
+        <v>161.034200441859</v>
       </c>
     </row>
     <row r="8">
@@ -579,7 +579,7 @@
         </is>
       </c>
       <c r="B10" t="n">
-        <v>0.3131680019583278</v>
+        <v>0.296825660738558</v>
       </c>
     </row>
     <row r="11">
@@ -589,7 +589,7 @@
         </is>
       </c>
       <c r="B11" s="5" t="n">
-        <v>45693.45306052222</v>
+        <v>45699.67276428798</v>
       </c>
     </row>
   </sheetData>
@@ -623,7 +623,7 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>-0.01209257954839928</v>
+        <v>-0.0120889506420294</v>
       </c>
     </row>
     <row r="3">
@@ -643,7 +643,7 @@
         </is>
       </c>
       <c r="B4" t="n">
-        <v>-1.000000003150307e-10</v>
+        <v>-1.000000000078997e-10</v>
       </c>
     </row>
     <row r="5">
@@ -653,7 +653,7 @@
         </is>
       </c>
       <c r="B5" t="n">
-        <v>10.32451578541716</v>
+        <v>9.66801273822297</v>
       </c>
     </row>
     <row r="6">
@@ -663,7 +663,7 @@
         </is>
       </c>
       <c r="B6" t="n">
-        <v>3.944989845749684</v>
+        <v>3.87117962463416</v>
       </c>
     </row>
     <row r="7">
@@ -673,7 +673,7 @@
         </is>
       </c>
       <c r="B7" t="n">
-        <v>149.8930707096686</v>
+        <v>156.4718267698503</v>
       </c>
     </row>
     <row r="8">
@@ -705,7 +705,7 @@
         </is>
       </c>
       <c r="B10" t="n">
-        <v>0.9882906863397111</v>
+        <v>1.006512531444407</v>
       </c>
     </row>
     <row r="11">
@@ -715,7 +715,7 @@
         </is>
       </c>
       <c r="B11" s="5" t="n">
-        <v>45693.45238813657</v>
+        <v>45699.67202224537</v>
       </c>
     </row>
   </sheetData>
@@ -749,7 +749,7 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>-0.01610674302545319</v>
+        <v>-0.01606135392338998</v>
       </c>
     </row>
     <row r="3">
@@ -769,7 +769,7 @@
         </is>
       </c>
       <c r="B4" t="n">
-        <v>-6.799806529675068e-08</v>
+        <v>-7.475878774398771e-08</v>
       </c>
     </row>
     <row r="5">
@@ -779,7 +779,7 @@
         </is>
       </c>
       <c r="B5" t="n">
-        <v>12.0602275179542</v>
+        <v>12.18231555679064</v>
       </c>
     </row>
     <row r="6">
@@ -789,7 +789,7 @@
         </is>
       </c>
       <c r="B6" t="n">
-        <v>5.674326186300808</v>
+        <v>5.940654007156947</v>
       </c>
     </row>
     <row r="7">
@@ -799,7 +799,7 @@
         </is>
       </c>
       <c r="B7" t="n">
-        <v>167.146703427554</v>
+        <v>168.4933306795201</v>
       </c>
     </row>
     <row r="8">
@@ -831,7 +831,7 @@
         </is>
       </c>
       <c r="B10" t="n">
-        <v>0.3757701370740637</v>
+        <v>0.3534290661868898</v>
       </c>
     </row>
     <row r="11">
@@ -841,7 +841,7 @@
         </is>
       </c>
       <c r="B11" s="5" t="n">
-        <v>45693.45244799768</v>
+        <v>45699.67208886574</v>
       </c>
     </row>
   </sheetData>
@@ -875,7 +875,7 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>-0.01695983256952929</v>
+        <v>-0.01696256126314312</v>
       </c>
     </row>
     <row r="3">
@@ -895,7 +895,7 @@
         </is>
       </c>
       <c r="B4" t="n">
-        <v>-1.2492545714739e-06</v>
+        <v>-1.235461859764849e-06</v>
       </c>
     </row>
     <row r="5">
@@ -905,7 +905,7 @@
         </is>
       </c>
       <c r="B5" t="n">
-        <v>11.51822269139612</v>
+        <v>11.68767004865758</v>
       </c>
     </row>
     <row r="6">
@@ -915,7 +915,7 @@
         </is>
       </c>
       <c r="B6" t="n">
-        <v>6.656630403651368</v>
+        <v>6.51982840267387</v>
       </c>
     </row>
     <row r="7">
@@ -925,7 +925,7 @@
         </is>
       </c>
       <c r="B7" t="n">
-        <v>166.1262270986385</v>
+        <v>164.8042277843232</v>
       </c>
     </row>
     <row r="8">
@@ -957,7 +957,7 @@
         </is>
       </c>
       <c r="B10" t="n">
-        <v>0.2948989181680448</v>
+        <v>0.261798062501053</v>
       </c>
     </row>
     <row r="11">
@@ -967,7 +967,7 @@
         </is>
       </c>
       <c r="B11" s="5" t="n">
-        <v>45693.4525119213</v>
+        <v>45699.67217222222</v>
       </c>
     </row>
   </sheetData>
@@ -1001,7 +1001,7 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>-0.01248343958520257</v>
+        <v>-0.01274294607116233</v>
       </c>
     </row>
     <row r="3">
@@ -1021,7 +1021,7 @@
         </is>
       </c>
       <c r="B4" t="n">
-        <v>-1.289118229116977e-06</v>
+        <v>-1.186117429086021e-06</v>
       </c>
     </row>
     <row r="5">
@@ -1031,7 +1031,7 @@
         </is>
       </c>
       <c r="B5" t="n">
-        <v>10.26618476607179</v>
+        <v>9.638138853111498</v>
       </c>
     </row>
     <row r="6">
@@ -1041,7 +1041,7 @@
         </is>
       </c>
       <c r="B6" t="n">
-        <v>2.154328457546242</v>
+        <v>1.719584105432685</v>
       </c>
     </row>
     <row r="7">
@@ -1051,7 +1051,7 @@
         </is>
       </c>
       <c r="B7" t="n">
-        <v>161.1335565471412</v>
+        <v>161.1720462889251</v>
       </c>
     </row>
     <row r="8">
@@ -1083,7 +1083,7 @@
         </is>
       </c>
       <c r="B10" t="n">
-        <v>0.7032549427593687</v>
+        <v>0.679415172045599</v>
       </c>
     </row>
     <row r="11">
@@ -1093,7 +1093,7 @@
         </is>
       </c>
       <c r="B11" s="5" t="n">
-        <v>45693.45258097223</v>
+        <v>45699.67224761574</v>
       </c>
     </row>
   </sheetData>
@@ -1127,7 +1127,7 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>-0.03456281175482238</v>
+        <v>-0.03171207709568124</v>
       </c>
     </row>
     <row r="3">
@@ -1147,7 +1147,7 @@
         </is>
       </c>
       <c r="B4" t="n">
-        <v>-1.17326381891609e-06</v>
+        <v>-6.640808991888091e-07</v>
       </c>
     </row>
     <row r="5">
@@ -1157,7 +1157,7 @@
         </is>
       </c>
       <c r="B5" t="n">
-        <v>13.07242886253713</v>
+        <v>13.12457404819691</v>
       </c>
     </row>
     <row r="6">
@@ -1167,7 +1167,7 @@
         </is>
       </c>
       <c r="B6" t="n">
-        <v>3.945584200254742</v>
+        <v>4.850793108584173</v>
       </c>
     </row>
     <row r="7">
@@ -1177,7 +1177,7 @@
         </is>
       </c>
       <c r="B7" t="n">
-        <v>183.8841247219519</v>
+        <v>192.7822173236272</v>
       </c>
     </row>
     <row r="8">
@@ -1209,7 +1209,7 @@
         </is>
       </c>
       <c r="B10" t="n">
-        <v>0.4721237144031179</v>
+        <v>0.4035749656714804</v>
       </c>
     </row>
     <row r="11">
@@ -1219,7 +1219,7 @@
         </is>
       </c>
       <c r="B11" s="5" t="n">
-        <v>45693.45262353009</v>
+        <v>45699.67230025463</v>
       </c>
     </row>
   </sheetData>
@@ -1253,7 +1253,7 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>-0.01226498829582623</v>
+        <v>-0.01217774837051229</v>
       </c>
     </row>
     <row r="3">
@@ -1273,7 +1273,7 @@
         </is>
       </c>
       <c r="B4" t="n">
-        <v>-9.628575086073408e-07</v>
+        <v>-7.539840963555597e-07</v>
       </c>
     </row>
     <row r="5">
@@ -1283,7 +1283,7 @@
         </is>
       </c>
       <c r="B5" t="n">
-        <v>11.47904678264748</v>
+        <v>11.8920547605261</v>
       </c>
     </row>
     <row r="6">
@@ -1293,7 +1293,7 @@
         </is>
       </c>
       <c r="B6" t="n">
-        <v>6.07638861006919</v>
+        <v>6.732531389095854</v>
       </c>
     </row>
     <row r="7">
@@ -1303,7 +1303,7 @@
         </is>
       </c>
       <c r="B7" t="n">
-        <v>154.3896030882613</v>
+        <v>153.6475571887269</v>
       </c>
     </row>
     <row r="8">
@@ -1335,7 +1335,7 @@
         </is>
       </c>
       <c r="B10" t="n">
-        <v>0.1553323888550164</v>
+        <v>0.1330591400676031</v>
       </c>
     </row>
     <row r="11">
@@ -1345,7 +1345,7 @@
         </is>
       </c>
       <c r="B11" s="5" t="n">
-        <v>45693.45265922454</v>
+        <v>45699.67233880787</v>
       </c>
     </row>
   </sheetData>
@@ -1379,7 +1379,7 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>-0.01424561353379935</v>
+        <v>-0.0138499392906743</v>
       </c>
     </row>
     <row r="3">
@@ -1399,7 +1399,7 @@
         </is>
       </c>
       <c r="B4" t="n">
-        <v>-2.948902662802961e-07</v>
+        <v>-4.625187281881448e-07</v>
       </c>
     </row>
     <row r="5">
@@ -1409,7 +1409,7 @@
         </is>
       </c>
       <c r="B5" t="n">
-        <v>12.98193427849214</v>
+        <v>13.10382884366287</v>
       </c>
     </row>
     <row r="6">
@@ -1419,7 +1419,7 @@
         </is>
       </c>
       <c r="B6" t="n">
-        <v>7.458301488077144</v>
+        <v>7.395463308394059</v>
       </c>
     </row>
     <row r="7">
@@ -1429,7 +1429,7 @@
         </is>
       </c>
       <c r="B7" t="n">
-        <v>156.3633455882561</v>
+        <v>156.2521507770053</v>
       </c>
     </row>
     <row r="8">
@@ -1461,7 +1461,7 @@
         </is>
       </c>
       <c r="B10" t="n">
-        <v>0.1772524972580675</v>
+        <v>0.187954995633264</v>
       </c>
     </row>
     <row r="11">
@@ -1471,7 +1471,7 @@
         </is>
       </c>
       <c r="B11" s="5" t="n">
-        <v>45693.45270262731</v>
+        <v>45699.67237949074</v>
       </c>
     </row>
   </sheetData>
@@ -1505,7 +1505,7 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>-0.01753618809312811</v>
+        <v>-0.01617768539418761</v>
       </c>
     </row>
     <row r="3">
@@ -1525,7 +1525,7 @@
         </is>
       </c>
       <c r="B4" t="n">
-        <v>-4.513928039973923e-07</v>
+        <v>-9.606638622740289e-07</v>
       </c>
     </row>
     <row r="5">
@@ -1535,7 +1535,7 @@
         </is>
       </c>
       <c r="B5" t="n">
-        <v>12.17380490732406</v>
+        <v>12.07726498676792</v>
       </c>
     </row>
     <row r="6">
@@ -1545,7 +1545,7 @@
         </is>
       </c>
       <c r="B6" t="n">
-        <v>7.527869582361509</v>
+        <v>7.101667672471773</v>
       </c>
     </row>
     <row r="7">
@@ -1555,7 +1555,7 @@
         </is>
       </c>
       <c r="B7" t="n">
-        <v>159.8940624678258</v>
+        <v>157.9393208305148</v>
       </c>
     </row>
     <row r="8">
@@ -1587,7 +1587,7 @@
         </is>
       </c>
       <c r="B10" t="n">
-        <v>0.2789154663958486</v>
+        <v>0.2764838304688362</v>
       </c>
     </row>
     <row r="11">
@@ -1597,7 +1597,7 @@
         </is>
       </c>
       <c r="B11" s="5" t="n">
-        <v>45693.4527422338</v>
+        <v>45699.67242075231</v>
       </c>
     </row>
   </sheetData>
@@ -1631,7 +1631,7 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>-0.01903642055713455</v>
+        <v>-0.01931196065975306</v>
       </c>
     </row>
     <row r="3">
@@ -1651,7 +1651,7 @@
         </is>
       </c>
       <c r="B4" t="n">
-        <v>-1.768510900403896e-06</v>
+        <v>-1.616479033324338e-06</v>
       </c>
     </row>
     <row r="5">
@@ -1661,7 +1661,7 @@
         </is>
       </c>
       <c r="B5" t="n">
-        <v>12.81055004721435</v>
+        <v>13.13675760359978</v>
       </c>
     </row>
     <row r="6">
@@ -1671,7 +1671,7 @@
         </is>
       </c>
       <c r="B6" t="n">
-        <v>6.089288318794379</v>
+        <v>5.950724724969729</v>
       </c>
     </row>
     <row r="7">
@@ -1681,7 +1681,7 @@
         </is>
       </c>
       <c r="B7" t="n">
-        <v>147.7461131275522</v>
+        <v>147.3773540818518</v>
       </c>
     </row>
     <row r="8">
@@ -1713,7 +1713,7 @@
         </is>
       </c>
       <c r="B10" t="n">
-        <v>0.6708960120216221</v>
+        <v>0.6576064579900261</v>
       </c>
     </row>
     <row r="11">
@@ -1723,7 +1723,7 @@
         </is>
       </c>
       <c r="B11" s="5" t="n">
-        <v>45693.45278238426</v>
+        <v>45699.6724678588</v>
       </c>
     </row>
   </sheetData>
@@ -1757,7 +1757,7 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>-0.03464213137223759</v>
+        <v>-0.02005139699079833</v>
       </c>
     </row>
     <row r="3">
@@ -1777,7 +1777,7 @@
         </is>
       </c>
       <c r="B4" t="n">
-        <v>-1.630795491819248e-06</v>
+        <v>-3.2867996690011e-06</v>
       </c>
     </row>
     <row r="5">
@@ -1787,7 +1787,7 @@
         </is>
       </c>
       <c r="B5" t="n">
-        <v>13.67921483785185</v>
+        <v>13.67428404704193</v>
       </c>
     </row>
     <row r="6">
@@ -1797,7 +1797,7 @@
         </is>
       </c>
       <c r="B6" t="n">
-        <v>3.063583936392551</v>
+        <v>4.915583932951407</v>
       </c>
     </row>
     <row r="7">
@@ -1807,7 +1807,7 @@
         </is>
       </c>
       <c r="B7" t="n">
-        <v>201.4001403837616</v>
+        <v>208.8997151189449</v>
       </c>
     </row>
     <row r="8">
@@ -1839,7 +1839,7 @@
         </is>
       </c>
       <c r="B10" t="n">
-        <v>0.2921983902880987</v>
+        <v>0.2816166117686612</v>
       </c>
     </row>
     <row r="11">
@@ -1849,7 +1849,7 @@
         </is>
       </c>
       <c r="B11" s="5" t="n">
-        <v>45693.45282216435</v>
+        <v>45699.67251216435</v>
       </c>
     </row>
   </sheetData>
@@ -1883,7 +1883,7 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>-0.01124300430680333</v>
+        <v>-0.01110803453187978</v>
       </c>
     </row>
     <row r="3">
@@ -1903,7 +1903,7 @@
         </is>
       </c>
       <c r="B4" t="n">
-        <v>-3.614832182316406e-07</v>
+        <v>-3.983342205357038e-07</v>
       </c>
     </row>
     <row r="5">
@@ -1913,7 +1913,7 @@
         </is>
       </c>
       <c r="B5" t="n">
-        <v>11.76782655258209</v>
+        <v>11.61306265065054</v>
       </c>
     </row>
     <row r="6">
@@ -1923,7 +1923,7 @@
         </is>
       </c>
       <c r="B6" t="n">
-        <v>5.178640830940104</v>
+        <v>5.258588144304044</v>
       </c>
     </row>
     <row r="7">
@@ -1933,7 +1933,7 @@
         </is>
       </c>
       <c r="B7" t="n">
-        <v>155.4426175049876</v>
+        <v>160.4912958158204</v>
       </c>
     </row>
     <row r="8">
@@ -1965,7 +1965,7 @@
         </is>
       </c>
       <c r="B10" t="n">
-        <v>0.279241594427752</v>
+        <v>0.2398145154032846</v>
       </c>
     </row>
     <row r="11">
@@ -1975,7 +1975,7 @@
         </is>
       </c>
       <c r="B11" s="5" t="n">
-        <v>45693.45188605324</v>
+        <v>45699.67143572916</v>
       </c>
     </row>
   </sheetData>
@@ -2009,7 +2009,7 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>-0.0307317280996529</v>
+        <v>-0.02500104128318027</v>
       </c>
     </row>
     <row r="3">
@@ -2029,7 +2029,7 @@
         </is>
       </c>
       <c r="B4" t="n">
-        <v>-8.729531749308279e-07</v>
+        <v>-5.135898872162277e-07</v>
       </c>
     </row>
     <row r="5">
@@ -2039,7 +2039,7 @@
         </is>
       </c>
       <c r="B5" t="n">
-        <v>11.86272102785905</v>
+        <v>12.05143632470478</v>
       </c>
     </row>
     <row r="6">
@@ -2049,7 +2049,7 @@
         </is>
       </c>
       <c r="B6" t="n">
-        <v>4.959174812592985</v>
+        <v>6.072419811520017</v>
       </c>
     </row>
     <row r="7">
@@ -2059,7 +2059,7 @@
         </is>
       </c>
       <c r="B7" t="n">
-        <v>163.1677667383437</v>
+        <v>164.4690201006416</v>
       </c>
     </row>
     <row r="8">
@@ -2091,7 +2091,7 @@
         </is>
       </c>
       <c r="B10" t="n">
-        <v>0.3384806329666538</v>
+        <v>0.286387786735651</v>
       </c>
     </row>
     <row r="11">
@@ -2101,7 +2101,7 @@
         </is>
       </c>
       <c r="B11" s="5" t="n">
-        <v>45693.45286032408</v>
+        <v>45699.67255212963</v>
       </c>
     </row>
   </sheetData>
@@ -2135,7 +2135,7 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>-0.01332271162033321</v>
+        <v>-0.01309579322349816</v>
       </c>
     </row>
     <row r="3">
@@ -2165,7 +2165,7 @@
         </is>
       </c>
       <c r="B5" t="n">
-        <v>12.63675001236583</v>
+        <v>12.43576456492437</v>
       </c>
     </row>
     <row r="6">
@@ -2175,7 +2175,7 @@
         </is>
       </c>
       <c r="B6" t="n">
-        <v>6.291420105410477</v>
+        <v>6.177438809527719</v>
       </c>
     </row>
     <row r="7">
@@ -2185,7 +2185,7 @@
         </is>
       </c>
       <c r="B7" t="n">
-        <v>152.6653355268988</v>
+        <v>153.2108751751385</v>
       </c>
     </row>
     <row r="8">
@@ -2217,7 +2217,7 @@
         </is>
       </c>
       <c r="B10" t="n">
-        <v>0.2023585012708984</v>
+        <v>0.19227165956517</v>
       </c>
     </row>
     <row r="11">
@@ -2227,7 +2227,7 @@
         </is>
       </c>
       <c r="B11" s="5" t="n">
-        <v>45693.45290096065</v>
+        <v>45699.67259806713</v>
       </c>
     </row>
   </sheetData>
@@ -2261,7 +2261,7 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>-0.01154269441922702</v>
+        <v>-0.01158812065812325</v>
       </c>
     </row>
     <row r="3">
@@ -2281,7 +2281,7 @@
         </is>
       </c>
       <c r="B4" t="n">
-        <v>-5.005834300896237e-07</v>
+        <v>-3.938757397830367e-07</v>
       </c>
     </row>
     <row r="5">
@@ -2291,7 +2291,7 @@
         </is>
       </c>
       <c r="B5" t="n">
-        <v>12.10879048092163</v>
+        <v>12.29506440822717</v>
       </c>
     </row>
     <row r="6">
@@ -2301,7 +2301,7 @@
         </is>
       </c>
       <c r="B6" t="n">
-        <v>4.553761714994808</v>
+        <v>5.031208770376971</v>
       </c>
     </row>
     <row r="7">
@@ -2311,7 +2311,7 @@
         </is>
       </c>
       <c r="B7" t="n">
-        <v>149.7779379858966</v>
+        <v>144.8491858156742</v>
       </c>
     </row>
     <row r="8">
@@ -2343,7 +2343,7 @@
         </is>
       </c>
       <c r="B10" t="n">
-        <v>0.235673736705289</v>
+        <v>0.2258624216083131</v>
       </c>
     </row>
     <row r="11">
@@ -2353,7 +2353,7 @@
         </is>
       </c>
       <c r="B11" s="5" t="n">
-        <v>45693.45294318287</v>
+        <v>45699.67263927084</v>
       </c>
     </row>
   </sheetData>
@@ -2387,7 +2387,7 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>-0.01406320970185783</v>
+        <v>-0.01385809094989918</v>
       </c>
     </row>
     <row r="3">
@@ -2407,7 +2407,7 @@
         </is>
       </c>
       <c r="B4" t="n">
-        <v>-4.608181352545496e-07</v>
+        <v>-3.741895442759716e-07</v>
       </c>
     </row>
     <row r="5">
@@ -2417,7 +2417,7 @@
         </is>
       </c>
       <c r="B5" t="n">
-        <v>12.0774177547363</v>
+        <v>12.28859336398036</v>
       </c>
     </row>
     <row r="6">
@@ -2427,7 +2427,7 @@
         </is>
       </c>
       <c r="B6" t="n">
-        <v>6.938337313852026</v>
+        <v>7.325898834286132</v>
       </c>
     </row>
     <row r="7">
@@ -2437,7 +2437,7 @@
         </is>
       </c>
       <c r="B7" t="n">
-        <v>159.4136743239206</v>
+        <v>159.9939862223962</v>
       </c>
     </row>
     <row r="8">
@@ -2469,7 +2469,7 @@
         </is>
       </c>
       <c r="B10" t="n">
-        <v>0.4972095002099772</v>
+        <v>0.2219323447089247</v>
       </c>
     </row>
     <row r="11">
@@ -2479,7 +2479,7 @@
         </is>
       </c>
       <c r="B11" s="5" t="n">
-        <v>45693.4529815162</v>
+        <v>45699.67267927084</v>
       </c>
     </row>
   </sheetData>
@@ -2513,7 +2513,7 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>-0.01420629455771528</v>
+        <v>-0.01394070698381442</v>
       </c>
     </row>
     <row r="3">
@@ -2533,7 +2533,7 @@
         </is>
       </c>
       <c r="B4" t="n">
-        <v>-1e-10</v>
+        <v>-1.000000000000517e-10</v>
       </c>
     </row>
     <row r="5">
@@ -2543,7 +2543,7 @@
         </is>
       </c>
       <c r="B5" t="n">
-        <v>11.99260469711941</v>
+        <v>11.98984461152882</v>
       </c>
     </row>
     <row r="6">
@@ -2553,7 +2553,7 @@
         </is>
       </c>
       <c r="B6" t="n">
-        <v>7.281800288123247</v>
+        <v>7.167725488565238</v>
       </c>
     </row>
     <row r="7">
@@ -2563,7 +2563,7 @@
         </is>
       </c>
       <c r="B7" t="n">
-        <v>154.515935508357</v>
+        <v>155.167126904195</v>
       </c>
     </row>
     <row r="8">
@@ -2595,7 +2595,7 @@
         </is>
       </c>
       <c r="B10" t="n">
-        <v>0.2299086452675216</v>
+        <v>0.2571575459472458</v>
       </c>
     </row>
     <row r="11">
@@ -2605,7 +2605,7 @@
         </is>
       </c>
       <c r="B11" s="5" t="n">
-        <v>45693.45302091435</v>
+        <v>45699.67272045139</v>
       </c>
     </row>
   </sheetData>
@@ -2639,7 +2639,7 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>-0.01123909411778164</v>
+        <v>-0.01106984620998736</v>
       </c>
     </row>
     <row r="3">
@@ -2659,7 +2659,7 @@
         </is>
       </c>
       <c r="B4" t="n">
-        <v>-1.452545007006024e-07</v>
+        <v>-1.879784379687332e-07</v>
       </c>
     </row>
     <row r="5">
@@ -2669,7 +2669,7 @@
         </is>
       </c>
       <c r="B5" t="n">
-        <v>12.47177950695337</v>
+        <v>12.39714713199219</v>
       </c>
     </row>
     <row r="6">
@@ -2679,7 +2679,7 @@
         </is>
       </c>
       <c r="B6" t="n">
-        <v>4.663760744826497</v>
+        <v>4.943663196731656</v>
       </c>
     </row>
     <row r="7">
@@ -2689,7 +2689,7 @@
         </is>
       </c>
       <c r="B7" t="n">
-        <v>176.4528501407135</v>
+        <v>177.6318041255628</v>
       </c>
     </row>
     <row r="8">
@@ -2721,7 +2721,7 @@
         </is>
       </c>
       <c r="B10" t="n">
-        <v>0.3531270122209433</v>
+        <v>0.3475518427219827</v>
       </c>
     </row>
     <row r="11">
@@ -2731,7 +2731,7 @@
         </is>
       </c>
       <c r="B11" s="5" t="n">
-        <v>45693.45194497685</v>
+        <v>45699.67150008102</v>
       </c>
     </row>
   </sheetData>
@@ -2765,7 +2765,7 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>-0.01631986209421345</v>
+        <v>-0.01622926636488082</v>
       </c>
     </row>
     <row r="3">
@@ -2785,7 +2785,7 @@
         </is>
       </c>
       <c r="B4" t="n">
-        <v>-2.392505664629136e-07</v>
+        <v>-2.638228465913171e-07</v>
       </c>
     </row>
     <row r="5">
@@ -2795,7 +2795,7 @@
         </is>
       </c>
       <c r="B5" t="n">
-        <v>11.90278996666389</v>
+        <v>12.16546815094099</v>
       </c>
     </row>
     <row r="6">
@@ -2805,7 +2805,7 @@
         </is>
       </c>
       <c r="B6" t="n">
-        <v>6.580046698235992</v>
+        <v>6.680023662096612</v>
       </c>
     </row>
     <row r="7">
@@ -2815,7 +2815,7 @@
         </is>
       </c>
       <c r="B7" t="n">
-        <v>172.6099944851552</v>
+        <v>173.6923360010707</v>
       </c>
     </row>
     <row r="8">
@@ -2847,7 +2847,7 @@
         </is>
       </c>
       <c r="B10" t="n">
-        <v>0.3408646095533109</v>
+        <v>0.2997107102016596</v>
       </c>
     </row>
     <row r="11">
@@ -2857,7 +2857,7 @@
         </is>
       </c>
       <c r="B11" s="5" t="n">
-        <v>45693.45200429398</v>
+        <v>45699.67156946759</v>
       </c>
     </row>
   </sheetData>
@@ -2891,7 +2891,7 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>-0.01239761331021841</v>
+        <v>-0.01248680672979542</v>
       </c>
     </row>
     <row r="3">
@@ -2911,7 +2911,7 @@
         </is>
       </c>
       <c r="B4" t="n">
-        <v>-6.700317054947346e-07</v>
+        <v>-5.954965802022144e-07</v>
       </c>
     </row>
     <row r="5">
@@ -2921,7 +2921,7 @@
         </is>
       </c>
       <c r="B5" t="n">
-        <v>11.27228363448384</v>
+        <v>11.12271950505708</v>
       </c>
     </row>
     <row r="6">
@@ -2931,7 +2931,7 @@
         </is>
       </c>
       <c r="B6" t="n">
-        <v>5.782142266894189</v>
+        <v>5.837740357183921</v>
       </c>
     </row>
     <row r="7">
@@ -2941,7 +2941,7 @@
         </is>
       </c>
       <c r="B7" t="n">
-        <v>171.6700782251175</v>
+        <v>173.2577859748561</v>
       </c>
     </row>
     <row r="8">
@@ -2973,7 +2973,7 @@
         </is>
       </c>
       <c r="B10" t="n">
-        <v>0.4685268080445136</v>
+        <v>0.4171146902939639</v>
       </c>
     </row>
     <row r="11">
@@ -2983,7 +2983,7 @@
         </is>
       </c>
       <c r="B11" s="5" t="n">
-        <v>45693.45206785879</v>
+        <v>45699.6716484375</v>
       </c>
     </row>
   </sheetData>
@@ -3017,7 +3017,7 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>-0.01399779096374016</v>
+        <v>-0.01402050783430401</v>
       </c>
     </row>
     <row r="3">
@@ -3037,7 +3037,7 @@
         </is>
       </c>
       <c r="B4" t="n">
-        <v>-3.708219592981682e-07</v>
+        <v>-3.506328900881021e-07</v>
       </c>
     </row>
     <row r="5">
@@ -3047,7 +3047,7 @@
         </is>
       </c>
       <c r="B5" t="n">
-        <v>11.17591586715134</v>
+        <v>10.76685570162649</v>
       </c>
     </row>
     <row r="6">
@@ -3057,7 +3057,7 @@
         </is>
       </c>
       <c r="B6" t="n">
-        <v>4.516618766192607</v>
+        <v>4.116564695636098</v>
       </c>
     </row>
     <row r="7">
@@ -3067,7 +3067,7 @@
         </is>
       </c>
       <c r="B7" t="n">
-        <v>183.2192030332556</v>
+        <v>180.5299384022</v>
       </c>
     </row>
     <row r="8">
@@ -3099,7 +3099,7 @@
         </is>
       </c>
       <c r="B10" t="n">
-        <v>0.4536983836113428</v>
+        <v>0.4416526914467693</v>
       </c>
     </row>
     <row r="11">
@@ -3109,7 +3109,7 @@
         </is>
       </c>
       <c r="B11" s="5" t="n">
-        <v>45693.45213512731</v>
+        <v>45699.67173180555</v>
       </c>
     </row>
   </sheetData>
@@ -3143,7 +3143,7 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>-0.01788690389135836</v>
+        <v>-0.01784971263347368</v>
       </c>
     </row>
     <row r="3">
@@ -3163,7 +3163,7 @@
         </is>
       </c>
       <c r="B4" t="n">
-        <v>-4.874692798017833e-07</v>
+        <v>-3.572199002878696e-07</v>
       </c>
     </row>
     <row r="5">
@@ -3173,7 +3173,7 @@
         </is>
       </c>
       <c r="B5" t="n">
-        <v>11.93478419950437</v>
+        <v>11.26171424391456</v>
       </c>
     </row>
     <row r="6">
@@ -3183,7 +3183,7 @@
         </is>
       </c>
       <c r="B6" t="n">
-        <v>3.886722855687176</v>
+        <v>3.431763141014778</v>
       </c>
     </row>
     <row r="7">
@@ -3193,7 +3193,7 @@
         </is>
       </c>
       <c r="B7" t="n">
-        <v>186.9396839790678</v>
+        <v>170.135032131336</v>
       </c>
     </row>
     <row r="8">
@@ -3225,7 +3225,7 @@
         </is>
       </c>
       <c r="B10" t="n">
-        <v>0.9088808132057458</v>
+        <v>0.8847618532295183</v>
       </c>
     </row>
     <row r="11">
@@ -3235,7 +3235,7 @@
         </is>
       </c>
       <c r="B11" s="5" t="n">
-        <v>45693.45220061343</v>
+        <v>45699.67179962963</v>
       </c>
     </row>
   </sheetData>
@@ -3269,7 +3269,7 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>-0.008860541720424392</v>
+        <v>-0.008807360459548873</v>
       </c>
     </row>
     <row r="3">
@@ -3289,7 +3289,7 @@
         </is>
       </c>
       <c r="B4" t="n">
-        <v>-7.679606681606496e-08</v>
+        <v>-8.824247661175542e-08</v>
       </c>
     </row>
     <row r="5">
@@ -3299,7 +3299,7 @@
         </is>
       </c>
       <c r="B5" t="n">
-        <v>10.36177053417512</v>
+        <v>10.31238609600846</v>
       </c>
     </row>
     <row r="6">
@@ -3309,7 +3309,7 @@
         </is>
       </c>
       <c r="B6" t="n">
-        <v>3.988679541161126</v>
+        <v>3.967781928581281</v>
       </c>
     </row>
     <row r="7">
@@ -3319,7 +3319,7 @@
         </is>
       </c>
       <c r="B7" t="n">
-        <v>177.1556637189054</v>
+        <v>177.4547622180878</v>
       </c>
     </row>
     <row r="8">
@@ -3351,7 +3351,7 @@
         </is>
       </c>
       <c r="B10" t="n">
-        <v>0.7420676939615982</v>
+        <v>0.3730107261709022</v>
       </c>
     </row>
     <row r="11">
@@ -3361,7 +3361,7 @@
         </is>
       </c>
       <c r="B11" s="5" t="n">
-        <v>45693.45226497686</v>
+        <v>45699.67187059027</v>
       </c>
     </row>
   </sheetData>
@@ -3395,7 +3395,7 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>-0.01283747420915961</v>
+        <v>-0.01279396309175958</v>
       </c>
     </row>
     <row r="3">
@@ -3415,7 +3415,7 @@
         </is>
       </c>
       <c r="B4" t="n">
-        <v>-6.544489253528912e-07</v>
+        <v>-6.780263453958441e-07</v>
       </c>
     </row>
     <row r="5">
@@ -3425,7 +3425,7 @@
         </is>
       </c>
       <c r="B5" t="n">
-        <v>11.55597505827869</v>
+        <v>11.54835232707443</v>
       </c>
     </row>
     <row r="6">
@@ -3435,7 +3435,7 @@
         </is>
       </c>
       <c r="B6" t="n">
-        <v>5.456717855944046</v>
+        <v>5.488265241023941</v>
       </c>
     </row>
     <row r="7">
@@ -3445,7 +3445,7 @@
         </is>
       </c>
       <c r="B7" t="n">
-        <v>176.2713124347164</v>
+        <v>177.3975175370383</v>
       </c>
     </row>
     <row r="8">
@@ -3477,7 +3477,7 @@
         </is>
       </c>
       <c r="B10" t="n">
-        <v>0.2603551200072844</v>
+        <v>0.2576582829884954</v>
       </c>
     </row>
     <row r="11">
@@ -3487,7 +3487,7 @@
         </is>
       </c>
       <c r="B11" s="5" t="n">
-        <v>45693.45233523148</v>
+        <v>45699.67196149306</v>
       </c>
     </row>
   </sheetData>

</xml_diff>